<commit_message>
Update values and report
</commit_message>
<xml_diff>
--- a/weekly/2025-CW01_weight_tracking.xlsx
+++ b/weekly/2025-CW01_weight_tracking.xlsx
@@ -483,19 +483,15 @@
       <c r="A2" s="2" t="n">
         <v>45884</v>
       </c>
-      <c r="B2" t="n">
-        <v>109</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>109.8</v>
+        <v>109.6</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>29</v>
       </c>
-      <c r="F2" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -515,9 +511,7 @@
       <c r="E3" t="n">
         <v>27.9</v>
       </c>
-      <c r="F3" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
     </row>
@@ -537,9 +531,7 @@
       <c r="E4" t="n">
         <v>28.8</v>
       </c>
-      <c r="F4" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
     </row>
@@ -548,20 +540,18 @@
         <v>45887</v>
       </c>
       <c r="B5" t="n">
-        <v>107.9</v>
+        <v>107.95</v>
       </c>
       <c r="C5" t="n">
         <v>108.8</v>
       </c>
       <c r="D5" t="n">
-        <v>30.7</v>
+        <v>30.55</v>
       </c>
       <c r="E5" t="n">
         <v>27.9</v>
       </c>
-      <c r="F5" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
     </row>
@@ -581,9 +571,7 @@
       <c r="E6" t="n">
         <v>29.5</v>
       </c>
-      <c r="F6" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
     </row>
@@ -603,9 +591,7 @@
       <c r="E7" t="n">
         <v>27.7</v>
       </c>
-      <c r="F7" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
     </row>
@@ -623,14 +609,10 @@
         <v>30.4</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
+        <v>28.9</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>